<commit_message>
modified:   README.md 	modified:   code.ipynb 	new file:   requirements.txt 	new file:   "results/\350\200\225\345\234\260\351\235\242\347\247\257\345\210\206\345\270\203\351\245\274\345\233\276.png" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/1-1-1.png" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/1-2-1.png" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/1-2-2.png" 	new file:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/2-2-1.png" 	modified:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/\351\231\204\344\273\2661.xlsx" 	modified:   "\351\242\230\347\233\256\345\217\212\351\231\204\344\273\266/\351\231\204\344\273\2662.xlsx"
</commit_message>
<xml_diff>
--- a/题目及附件/附件2.xlsx
+++ b/题目及附件/附件2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2024-5-1\数学建模竞赛组委会、专家组工作\竞赛2024\C题乡村农作物种植策略优化\2024-8-28-1 C题(蔡志杰)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Math_model\CUMCM2024Problems\C题\题目及附件\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C5F6CD-59CD-4C72-91B3-4A313A138E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010"/>
+    <workbookView xWindow="2340" yWindow="4170" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023年的农作物种植情况" sheetId="4" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="229">
   <si>
     <t>6.00-8.00</t>
   </si>
@@ -1996,69 +1997,6 @@
         <charset val="134"/>
       </rPr>
       <t>第二季</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>注：</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(1) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>该数据是</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2023</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>年根据近几年的相应数据统计所得。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(2) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>智慧大棚第一季可种植的蔬菜作物及其亩产量、种植成本和销售价格均与普通大棚相同，表中省略。</t>
     </r>
   </si>
   <si>
@@ -2197,8 +2135,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2307,13 +2245,6 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -2430,7 +2361,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2494,42 +2425,36 @@
     <xf numFmtId="57" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1"/>
-    <cellStyle name="常规 27" xfId="2"/>
-    <cellStyle name="常规 34" xfId="3"/>
+    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="常规 27" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规 34" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2830,13 +2755,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2856,7 +2781,7 @@
       <c r="C1" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>197</v>
       </c>
       <c r="E1" s="18" t="s">
@@ -3387,7 +3312,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="4">
@@ -3407,7 +3332,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="4">
         <v>36</v>
       </c>
@@ -3425,7 +3350,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4">
@@ -3445,7 +3370,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="4">
         <v>35</v>
       </c>
@@ -3463,7 +3388,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="4">
@@ -3483,7 +3408,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="4">
         <v>35</v>
       </c>
@@ -3501,7 +3426,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="4">
@@ -3521,7 +3446,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="4">
         <v>35</v>
       </c>
@@ -3539,7 +3464,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B36" s="4">
@@ -3559,7 +3484,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="4">
         <v>36</v>
       </c>
@@ -3577,7 +3502,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="26" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="4">
@@ -3597,7 +3522,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="4">
         <v>37</v>
       </c>
@@ -3655,7 +3580,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>94</v>
       </c>
       <c r="B42" s="4">
@@ -3675,7 +3600,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="4">
         <v>38</v>
       </c>
@@ -3693,7 +3618,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B44" s="4">
@@ -3713,7 +3638,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="4">
         <v>38</v>
       </c>
@@ -3731,7 +3656,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B46" s="4">
@@ -3751,7 +3676,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="4">
         <v>38</v>
       </c>
@@ -3769,7 +3694,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B48" s="4">
@@ -3789,7 +3714,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="4">
         <v>39</v>
       </c>
@@ -3807,7 +3732,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+      <c r="A50" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B50" s="4">
@@ -3827,7 +3752,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="4">
         <v>39</v>
       </c>
@@ -3845,7 +3770,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="26" t="s">
         <v>97</v>
       </c>
       <c r="B52" s="4">
@@ -3865,7 +3790,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="4">
         <v>39</v>
       </c>
@@ -3883,7 +3808,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B54" s="4">
@@ -3903,7 +3828,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="4">
         <v>40</v>
       </c>
@@ -3921,7 +3846,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B56" s="4">
@@ -3941,7 +3866,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
+      <c r="A57" s="27"/>
       <c r="B57" s="4">
         <v>40</v>
       </c>
@@ -3959,7 +3884,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B58" s="4">
@@ -3979,7 +3904,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="4">
         <v>40</v>
       </c>
@@ -3997,7 +3922,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="26" t="s">
         <v>100</v>
       </c>
       <c r="B60" s="4">
@@ -4017,7 +3942,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="4">
         <v>41</v>
       </c>
@@ -4035,7 +3960,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="4">
@@ -4055,7 +3980,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
+      <c r="A63" s="27"/>
       <c r="B63" s="4">
         <v>41</v>
       </c>
@@ -4073,7 +3998,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B64" s="4">
@@ -4093,7 +4018,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="4">
         <v>41</v>
       </c>
@@ -4111,7 +4036,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B66" s="4">
@@ -4131,7 +4056,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="4">
         <v>41</v>
       </c>
@@ -4149,7 +4074,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
+      <c r="A68" s="26" t="s">
         <v>104</v>
       </c>
       <c r="B68" s="4">
@@ -4169,7 +4094,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="30"/>
+      <c r="A69" s="27"/>
       <c r="B69" s="4">
         <v>41</v>
       </c>
@@ -4187,7 +4112,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B70" s="4">
@@ -4207,7 +4132,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="4">
         <v>27</v>
       </c>
@@ -4225,7 +4150,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
+      <c r="A72" s="27"/>
       <c r="B72" s="4">
         <v>41</v>
       </c>
@@ -4243,7 +4168,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B73" s="4">
@@ -4263,7 +4188,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="4">
         <v>41</v>
       </c>
@@ -4281,7 +4206,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="28" t="s">
+      <c r="A75" s="26" t="s">
         <v>105</v>
       </c>
       <c r="B75" s="4">
@@ -4301,7 +4226,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="4">
         <v>33</v>
       </c>
@@ -4319,7 +4244,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="4">
         <v>24</v>
       </c>
@@ -4337,7 +4262,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="30"/>
+      <c r="A78" s="27"/>
       <c r="B78" s="4">
         <v>21</v>
       </c>
@@ -4355,7 +4280,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="28" t="s">
+      <c r="A79" s="26" t="s">
         <v>106</v>
       </c>
       <c r="B79" s="4">
@@ -4375,7 +4300,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
+      <c r="A80" s="28"/>
       <c r="B80" s="4">
         <v>26</v>
       </c>
@@ -4393,7 +4318,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="4">
         <v>22</v>
       </c>
@@ -4411,7 +4336,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="4">
         <v>29</v>
       </c>
@@ -4429,7 +4354,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
+      <c r="A83" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B83" s="4">
@@ -4449,7 +4374,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="4">
         <v>28</v>
       </c>
@@ -4467,7 +4392,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="30"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="4">
         <v>30</v>
       </c>
@@ -4485,7 +4410,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="28" t="s">
+      <c r="A86" s="26" t="s">
         <v>133</v>
       </c>
       <c r="B86" s="4">
@@ -4505,7 +4430,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="4">
         <v>34</v>
       </c>
@@ -4523,7 +4448,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="4">
         <v>23</v>
       </c>
@@ -4542,12 +4467,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A70:A72"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A64:A65"/>
@@ -4563,11 +4487,12 @@
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4576,13 +4501,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I108" sqref="I108"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4617,10 +4544,10 @@
         <v>135</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.25">
@@ -7406,23 +7333,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
-        <v>227</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
-      <c r="B111" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A3:H109">
-    <sortCondition ref="A3:A109"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H108">
+    <sortCondition ref="A3:A108"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>